<commit_message>
fixed up ClueLayoutTests.xslx for the second time lol
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTests.xlsx
+++ b/data/ClueLayoutTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/burns_mines_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{8F1CACB8-1431-A54A-A4D2-8715BFAC834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D20232A-DA5C-F04D-8818-316FF792B712}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{8F1CACB8-1431-A54A-A4D2-8715BFAC834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9F1EFF5-4B91-7B4E-8DF1-B8047BD5B9B8}"/>
   <bookViews>
     <workbookView xWindow="-4940" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,9 +136,6 @@
     <t/>
   </si>
   <si>
-    <t>Number of Doors: 17</t>
-  </si>
-  <si>
     <t>Red: Test occupied</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Grey: Occupied/Door Direction Test</t>
+  </si>
+  <si>
+    <t>Number of Doors: 19</t>
   </si>
 </sst>
 </file>
@@ -666,7 +666,7 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3225,20 +3225,17 @@
         <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="1">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -3251,7 +3248,7 @@
     </row>
     <row r="31" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3261,7 +3258,7 @@
     </row>
     <row r="32" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -3269,7 +3266,7 @@
     </row>
     <row r="33" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
@@ -3277,7 +3274,7 @@
     </row>
     <row r="34" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>

</xml_diff>